<commit_message>
tech, goog, nvda updates
</commit_message>
<xml_diff>
--- a/NVDA/NVDA Model - (02-10-2024).xlsx
+++ b/NVDA/NVDA Model - (02-10-2024).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buzz5\OneDrive\Desktop\FModels\NVDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C0668AB-3E2F-4271-A90B-B2E81AC63C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F63BF6-BFBE-4F1B-84FA-A3C1F1ED54BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{86DED09B-2833-4D69-AD50-3DC99F242132}"/>
+    <workbookView xWindow="-22065" yWindow="2280" windowWidth="21600" windowHeight="11385" xr2:uid="{86DED09B-2833-4D69-AD50-3DC99F242132}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>ALL IN $ USD</t>
   </si>
@@ -319,6 +319,72 @@
   </si>
   <si>
     <t>Annual Reports:</t>
+  </si>
+  <si>
+    <t>NVIDIA is a semiconductor company based in Santa Clara, California. NVIDIA has made significant advancements in AI and DL through it's CUDA platform.</t>
+  </si>
+  <si>
+    <t>Founder and CEO of NVIDIA since inception</t>
+  </si>
+  <si>
+    <t>Bachelors Electrical Eng @ Oregon State</t>
+  </si>
+  <si>
+    <t>Masters EE Stanford</t>
+  </si>
+  <si>
+    <t>60 yrs old</t>
+  </si>
+  <si>
+    <t>owns 3.6% of company stock</t>
+  </si>
+  <si>
+    <t>21.36M yearly comp</t>
+  </si>
+  <si>
+    <t>Reneas</t>
+  </si>
+  <si>
+    <t>Cisco</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Broadcom</t>
+  </si>
+  <si>
+    <t>Intel</t>
+  </si>
+  <si>
+    <t>Qualcomm</t>
+  </si>
+  <si>
+    <t>M&amp;A:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mellanox </t>
+  </si>
+  <si>
+    <t>Arm</t>
+  </si>
+  <si>
+    <t>SwiftStack</t>
+  </si>
+  <si>
+    <t>Ageia</t>
+  </si>
+  <si>
+    <t>OmniML</t>
+  </si>
+  <si>
+    <t>CoreWeave</t>
+  </si>
+  <si>
+    <t>TSMC makes NVIDIA chips</t>
   </si>
 </sst>
 </file>
@@ -710,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A915255-7085-4C22-945C-1F53AB87465D}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,21 +787,21 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f ca="1">TODAY()</f>
-        <v>45332</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
@@ -746,7 +812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -756,16 +822,22 @@
       <c r="E4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -776,7 +848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
@@ -784,7 +856,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
@@ -792,7 +864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
@@ -800,7 +872,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
@@ -811,39 +883,59 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G16" s="3"/>
+      <c r="H16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>26</v>
       </c>
@@ -851,15 +943,22 @@
         <v>721</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="4">
         <v>2468</v>
       </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>28</v>
       </c>
@@ -867,24 +966,42 @@
         <f>E18*E17</f>
         <v>1779428</v>
       </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>101</v>
+      </c>
+      <c r="K19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>29</v>
       </c>
       <c r="E20" s="4">
         <v>13296</v>
       </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>30</v>
       </c>
       <c r="E21" s="4">
         <v>10605</v>
       </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>103</v>
+      </c>
+      <c r="K21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>31</v>
       </c>
@@ -892,16 +1009,28 @@
         <f>E19-E20+E21</f>
         <v>1776737</v>
       </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>104</v>
+      </c>
+      <c r="K22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>32</v>
       </c>
       <c r="E23" s="4">
         <v>22160</v>
       </c>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>105</v>
+      </c>
+      <c r="K23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>33</v>
       </c>
@@ -909,8 +1038,19 @@
         <f>E22/E23</f>
         <v>80.177662454873641</v>
       </c>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>106</v>
+      </c>
+      <c r="K24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D26" s="3" t="s">
         <v>34</v>
       </c>
@@ -927,11 +1067,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B207C8-9AB3-4D32-81A5-CB52CE47C6B0}">
   <dimension ref="A1:FH26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="AO5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="AA5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AX19" sqref="AX19"/>
+      <selection pane="bottomRight" activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,7 +1559,7 @@
         <v>92</v>
       </c>
       <c r="AI6" s="10">
-        <v>9.6000000000000002E-2</v>
+        <v>0.08</v>
       </c>
       <c r="AJ6" s="4"/>
       <c r="AK6" s="4"/>
@@ -1597,7 +1737,7 @@
         <v>1409</v>
       </c>
       <c r="AM7" s="4">
-        <f t="shared" ref="AM7:BE7" si="10">AM5-AM6</f>
+        <f t="shared" ref="AM7:AX7" si="10">AM5-AM6</f>
         <v>2059</v>
       </c>
       <c r="AN7" s="4">
@@ -1750,7 +1890,7 @@
       </c>
       <c r="AI8" s="4">
         <f>NPV(AI7,AL13:FH13)</f>
-        <v>1748733.2862451293</v>
+        <v>567665.79106775171</v>
       </c>
       <c r="AJ8" s="4"/>
       <c r="AK8" s="4"/>
@@ -1925,7 +2065,7 @@
       <c r="AJ9" s="4"/>
       <c r="AK9" s="4"/>
       <c r="AL9" s="4">
-        <f t="shared" ref="AL9:BE9" si="20">AL7-AL8</f>
+        <f t="shared" ref="AL9:AX9" si="20">AL7-AL8</f>
         <v>256</v>
       </c>
       <c r="AM9" s="4">
@@ -2082,7 +2222,7 @@
       </c>
       <c r="AI10" s="4">
         <f>AI8+AI9</f>
-        <v>1762029.2862451293</v>
+        <v>580961.79106775171</v>
       </c>
       <c r="AJ10" s="4"/>
       <c r="AK10" s="4"/>
@@ -2258,7 +2398,7 @@
       <c r="AJ11" s="4"/>
       <c r="AK11" s="4"/>
       <c r="AL11" s="4">
-        <f t="shared" ref="AL11:BE11" si="30">AL9+AL10</f>
+        <f t="shared" ref="AL11:AX11" si="30">AL9+AL10</f>
         <v>271</v>
       </c>
       <c r="AM11" s="4">
@@ -2585,12 +2725,12 @@
       </c>
       <c r="AI13" s="4">
         <f>AI10/Main!E18</f>
-        <v>713.95027805718371</v>
+        <v>235.39780837429163</v>
       </c>
       <c r="AJ13" s="4"/>
       <c r="AK13" s="4"/>
       <c r="AL13" s="4">
-        <f t="shared" ref="AL13:BE13" si="40">AL11-AL12</f>
+        <f t="shared" ref="AL13:AX13" si="40">AL11-AL12</f>
         <v>253</v>
       </c>
       <c r="AM13" s="4">
@@ -2643,459 +2783,459 @@
       </c>
       <c r="AY13" s="4">
         <f>AX13*($AI$6+1)</f>
-        <v>4787.3280000000004</v>
+        <v>4717.4400000000005</v>
       </c>
       <c r="AZ13" s="4">
         <f t="shared" ref="AZ13:DK13" si="41">AY13*($AI$6+1)</f>
-        <v>5246.9114880000006</v>
+        <v>5094.8352000000004</v>
       </c>
       <c r="BA13" s="4">
         <f t="shared" si="41"/>
-        <v>5750.6149908480011</v>
+        <v>5502.4220160000004</v>
       </c>
       <c r="BB13" s="4">
         <f t="shared" si="41"/>
-        <v>6302.6740299694093</v>
+        <v>5942.6157772800007</v>
       </c>
       <c r="BC13" s="4">
         <f t="shared" si="41"/>
-        <v>6907.7307368464735</v>
+        <v>6418.0250394624009</v>
       </c>
       <c r="BD13" s="4">
         <f t="shared" si="41"/>
-        <v>7570.872887583736</v>
+        <v>6931.4670426193934</v>
       </c>
       <c r="BE13" s="4">
         <f t="shared" si="41"/>
-        <v>8297.6766847917752</v>
+        <v>7485.9844060289452</v>
       </c>
       <c r="BF13" s="4">
         <f t="shared" si="41"/>
-        <v>9094.2536465317862</v>
+        <v>8084.8631585112616</v>
       </c>
       <c r="BG13" s="4">
         <f t="shared" si="41"/>
-        <v>9967.3019965988387</v>
+        <v>8731.652211192164</v>
       </c>
       <c r="BH13" s="4">
         <f t="shared" si="41"/>
-        <v>10924.162988272328</v>
+        <v>9430.1843880875385</v>
       </c>
       <c r="BI13" s="4">
         <f t="shared" si="41"/>
-        <v>11972.882635146472</v>
+        <v>10184.599139134541</v>
       </c>
       <c r="BJ13" s="4">
         <f t="shared" si="41"/>
-        <v>13122.279368120535</v>
+        <v>10999.367070265305</v>
       </c>
       <c r="BK13" s="4">
         <f t="shared" si="41"/>
-        <v>14382.018187460108</v>
+        <v>11879.316435886531</v>
       </c>
       <c r="BL13" s="4">
         <f t="shared" si="41"/>
-        <v>15762.691933456279</v>
+        <v>12829.661750757454</v>
       </c>
       <c r="BM13" s="4">
         <f t="shared" si="41"/>
-        <v>17275.910359068082</v>
+        <v>13856.034690818051</v>
       </c>
       <c r="BN13" s="4">
         <f t="shared" si="41"/>
-        <v>18934.397753538618</v>
+        <v>14964.517466083496</v>
       </c>
       <c r="BO13" s="4">
         <f t="shared" si="41"/>
-        <v>20752.099937878327</v>
+        <v>16161.678863370178</v>
       </c>
       <c r="BP13" s="4">
         <f t="shared" si="41"/>
-        <v>22744.301531914647</v>
+        <v>17454.613172439793</v>
       </c>
       <c r="BQ13" s="4">
         <f t="shared" si="41"/>
-        <v>24927.754478978455</v>
+        <v>18850.982226234977</v>
       </c>
       <c r="BR13" s="4">
         <f t="shared" si="41"/>
-        <v>27320.818908960387</v>
+        <v>20359.060804333778</v>
       </c>
       <c r="BS13" s="4">
         <f t="shared" si="41"/>
-        <v>29943.617524220586</v>
+        <v>21987.785668680481</v>
       </c>
       <c r="BT13" s="4">
         <f t="shared" si="41"/>
-        <v>32818.204806545764</v>
+        <v>23746.808522174921</v>
       </c>
       <c r="BU13" s="4">
         <f t="shared" si="41"/>
-        <v>35968.752467974162</v>
+        <v>25646.553203948915</v>
       </c>
       <c r="BV13" s="4">
         <f t="shared" si="41"/>
-        <v>39421.752704899685</v>
+        <v>27698.277460264831</v>
       </c>
       <c r="BW13" s="4">
         <f t="shared" si="41"/>
-        <v>43206.240964570061</v>
+        <v>29914.13965708602</v>
       </c>
       <c r="BX13" s="4">
         <f t="shared" si="41"/>
-        <v>47354.040097168792</v>
+        <v>32307.270829652902</v>
       </c>
       <c r="BY13" s="4">
         <f t="shared" si="41"/>
-        <v>51900.027946497001</v>
+        <v>34891.852496025138</v>
       </c>
       <c r="BZ13" s="4">
         <f t="shared" si="41"/>
-        <v>56882.430629360715</v>
+        <v>37683.20069570715</v>
       </c>
       <c r="CA13" s="4">
         <f t="shared" si="41"/>
-        <v>62343.143969779347</v>
+        <v>40697.856751363724</v>
       </c>
       <c r="CB13" s="4">
         <f t="shared" si="41"/>
-        <v>68328.085790878176</v>
+        <v>43953.685291472822</v>
       </c>
       <c r="CC13" s="4">
         <f t="shared" si="41"/>
-        <v>74887.582026802484</v>
+        <v>47469.980114790655</v>
       </c>
       <c r="CD13" s="4">
         <f t="shared" si="41"/>
-        <v>82076.789901375523</v>
+        <v>51267.578523973913</v>
       </c>
       <c r="CE13" s="4">
         <f t="shared" si="41"/>
-        <v>89956.161731907574</v>
+        <v>55368.984805891829</v>
       </c>
       <c r="CF13" s="4">
         <f t="shared" si="41"/>
-        <v>98591.953258170703</v>
+        <v>59798.50359036318</v>
       </c>
       <c r="CG13" s="4">
         <f t="shared" si="41"/>
-        <v>108056.7807709551</v>
+        <v>64582.383877592241</v>
       </c>
       <c r="CH13" s="4">
         <f t="shared" si="41"/>
-        <v>118430.2317249668</v>
+        <v>69748.974587799632</v>
       </c>
       <c r="CI13" s="4">
         <f t="shared" si="41"/>
-        <v>129799.53397056361</v>
+        <v>75328.892554823615</v>
       </c>
       <c r="CJ13" s="4">
         <f t="shared" si="41"/>
-        <v>142260.28923173773</v>
+        <v>81355.20395920951</v>
       </c>
       <c r="CK13" s="4">
         <f t="shared" si="41"/>
-        <v>155917.27699798456</v>
+        <v>87863.620275946276</v>
       </c>
       <c r="CL13" s="4">
         <f t="shared" si="41"/>
-        <v>170885.3355897911</v>
+        <v>94892.709898021989</v>
       </c>
       <c r="CM13" s="4">
         <f t="shared" si="41"/>
-        <v>187290.32780641105</v>
+        <v>102484.12668986376</v>
       </c>
       <c r="CN13" s="4">
         <f t="shared" si="41"/>
-        <v>205270.19927582651</v>
+        <v>110682.85682505286</v>
       </c>
       <c r="CO13" s="4">
         <f t="shared" si="41"/>
-        <v>224976.13840630586</v>
+        <v>119537.4853710571</v>
       </c>
       <c r="CP13" s="4">
         <f t="shared" si="41"/>
-        <v>246573.84769331125</v>
+        <v>129100.48420074169</v>
       </c>
       <c r="CQ13" s="4">
         <f t="shared" si="41"/>
-        <v>270244.93707186915</v>
+        <v>139428.52293680102</v>
       </c>
       <c r="CR13" s="4">
         <f t="shared" si="41"/>
-        <v>296188.45103076863</v>
+        <v>150582.80477174511</v>
       </c>
       <c r="CS13" s="4">
         <f t="shared" si="41"/>
-        <v>324622.54232972243</v>
+        <v>162629.42915348473</v>
       </c>
       <c r="CT13" s="4">
         <f t="shared" si="41"/>
-        <v>355786.30639337579</v>
+        <v>175639.78348576353</v>
       </c>
       <c r="CU13" s="4">
         <f t="shared" si="41"/>
-        <v>389941.79180713987</v>
+        <v>189690.96616462464</v>
       </c>
       <c r="CV13" s="4">
         <f t="shared" si="41"/>
-        <v>427376.20382062532</v>
+        <v>204866.24345779463</v>
       </c>
       <c r="CW13" s="4">
         <f t="shared" si="41"/>
-        <v>468404.31938740541</v>
+        <v>221255.54293441822</v>
       </c>
       <c r="CX13" s="4">
         <f t="shared" si="41"/>
-        <v>513371.13404859637</v>
+        <v>238955.9863691717</v>
       </c>
       <c r="CY13" s="4">
         <f t="shared" si="41"/>
-        <v>562654.76291726169</v>
+        <v>258072.46527870547</v>
       </c>
       <c r="CZ13" s="4">
         <f t="shared" si="41"/>
-        <v>616669.62015731889</v>
+        <v>278718.26250100194</v>
       </c>
       <c r="DA13" s="4">
         <f t="shared" si="41"/>
-        <v>675869.9036924215</v>
+        <v>301015.7235010821</v>
       </c>
       <c r="DB13" s="4">
         <f t="shared" si="41"/>
-        <v>740753.41444689408</v>
+        <v>325096.98138116871</v>
       </c>
       <c r="DC13" s="4">
         <f t="shared" si="41"/>
-        <v>811865.74223379593</v>
+        <v>351104.7398916622</v>
       </c>
       <c r="DD13" s="4">
         <f t="shared" si="41"/>
-        <v>889804.85348824039</v>
+        <v>379193.11908299522</v>
       </c>
       <c r="DE13" s="4">
         <f t="shared" si="41"/>
-        <v>975226.11942311155</v>
+        <v>409528.56860963488</v>
       </c>
       <c r="DF13" s="4">
         <f t="shared" si="41"/>
-        <v>1068847.8268877303</v>
+        <v>442290.85409840569</v>
       </c>
       <c r="DG13" s="4">
         <f t="shared" si="41"/>
-        <v>1171457.2182689526</v>
+        <v>477674.12242627819</v>
       </c>
       <c r="DH13" s="4">
         <f t="shared" si="41"/>
-        <v>1283917.1112227722</v>
+        <v>515888.05222038046</v>
       </c>
       <c r="DI13" s="4">
         <f t="shared" si="41"/>
-        <v>1407173.1539001584</v>
+        <v>557159.09639801097</v>
       </c>
       <c r="DJ13" s="4">
         <f t="shared" si="41"/>
-        <v>1542261.7766745738</v>
+        <v>601731.82410985185</v>
       </c>
       <c r="DK13" s="4">
         <f t="shared" si="41"/>
-        <v>1690318.907235333</v>
+        <v>649870.37003863999</v>
       </c>
       <c r="DL13" s="4">
         <f t="shared" ref="DL13:FH13" si="42">DK13*($AI$6+1)</f>
-        <v>1852589.5223299251</v>
+        <v>701859.99964173127</v>
       </c>
       <c r="DM13" s="4">
         <f t="shared" si="42"/>
-        <v>2030438.1164735982</v>
+        <v>758008.79961306986</v>
       </c>
       <c r="DN13" s="4">
         <f t="shared" si="42"/>
-        <v>2225360.1756550637</v>
+        <v>818649.50358211552</v>
       </c>
       <c r="DO13" s="4">
         <f t="shared" si="42"/>
-        <v>2438994.7525179498</v>
+        <v>884141.46386868483</v>
       </c>
       <c r="DP13" s="4">
         <f t="shared" si="42"/>
-        <v>2673138.248759673</v>
+        <v>954872.78097817965</v>
       </c>
       <c r="DQ13" s="4">
         <f t="shared" si="42"/>
-        <v>2929759.5206406019</v>
+        <v>1031262.6034564341</v>
       </c>
       <c r="DR13" s="4">
         <f t="shared" si="42"/>
-        <v>3211016.4346221001</v>
+        <v>1113763.6117329488</v>
       </c>
       <c r="DS13" s="4">
         <f t="shared" si="42"/>
-        <v>3519274.0123458221</v>
+        <v>1202864.7006715848</v>
       </c>
       <c r="DT13" s="4">
         <f t="shared" si="42"/>
-        <v>3857124.3175310213</v>
+        <v>1299093.8767253116</v>
       </c>
       <c r="DU13" s="4">
         <f t="shared" si="42"/>
-        <v>4227408.252014</v>
+        <v>1403021.3868633367</v>
       </c>
       <c r="DV13" s="4">
         <f t="shared" si="42"/>
-        <v>4633239.4442073442</v>
+        <v>1515263.0978124037</v>
       </c>
       <c r="DW13" s="4">
         <f t="shared" si="42"/>
-        <v>5078030.43085125</v>
+        <v>1636484.145637396</v>
       </c>
       <c r="DX13" s="4">
         <f t="shared" si="42"/>
-        <v>5565521.3522129701</v>
+        <v>1767402.8772883879</v>
       </c>
       <c r="DY13" s="4">
         <f t="shared" si="42"/>
-        <v>6099811.4020254156</v>
+        <v>1908795.1074714591</v>
       </c>
       <c r="DZ13" s="4">
         <f t="shared" si="42"/>
-        <v>6685393.2966198558</v>
+        <v>2061498.7160691759</v>
       </c>
       <c r="EA13" s="4">
         <f t="shared" si="42"/>
-        <v>7327191.0530953621</v>
+        <v>2226418.6133547099</v>
       </c>
       <c r="EB13" s="4">
         <f t="shared" si="42"/>
-        <v>8030601.3941925177</v>
+        <v>2404532.1024230868</v>
       </c>
       <c r="EC13" s="4">
         <f t="shared" si="42"/>
-        <v>8801539.1280349996</v>
+        <v>2596894.6706169341</v>
       </c>
       <c r="ED13" s="4">
         <f t="shared" si="42"/>
-        <v>9646486.8843263611</v>
+        <v>2804646.2442662888</v>
       </c>
       <c r="EE13" s="4">
         <f t="shared" si="42"/>
-        <v>10572549.625221692</v>
+        <v>3029017.9438075921</v>
       </c>
       <c r="EF13" s="4">
         <f t="shared" si="42"/>
-        <v>11587514.389242975</v>
+        <v>3271339.3793121995</v>
       </c>
       <c r="EG13" s="4">
         <f t="shared" si="42"/>
-        <v>12699915.770610301</v>
+        <v>3533046.5296571758</v>
       </c>
       <c r="EH13" s="4">
         <f t="shared" si="42"/>
-        <v>13919107.684588891</v>
+        <v>3815690.25202975</v>
       </c>
       <c r="EI13" s="4">
         <f t="shared" si="42"/>
-        <v>15255342.022309424</v>
+        <v>4120945.4721921305</v>
       </c>
       <c r="EJ13" s="4">
         <f t="shared" si="42"/>
-        <v>16719854.85645113</v>
+        <v>4450621.1099675009</v>
       </c>
       <c r="EK13" s="4">
         <f t="shared" si="42"/>
-        <v>18324960.922670439</v>
+        <v>4806670.7987649012</v>
       </c>
       <c r="EL13" s="4">
         <f t="shared" si="42"/>
-        <v>20084157.171246804</v>
+        <v>5191204.4626660934</v>
       </c>
       <c r="EM13" s="4">
         <f t="shared" si="42"/>
-        <v>22012236.2596865</v>
+        <v>5606500.8196793813</v>
       </c>
       <c r="EN13" s="4">
         <f t="shared" si="42"/>
-        <v>24125410.940616407</v>
+        <v>6055020.8852537321</v>
       </c>
       <c r="EO13" s="4">
         <f t="shared" si="42"/>
-        <v>26441450.390915584</v>
+        <v>6539422.5560740307</v>
       </c>
       <c r="EP13" s="4">
         <f t="shared" si="42"/>
-        <v>28979829.628443483</v>
+        <v>7062576.3605599534</v>
       </c>
       <c r="EQ13" s="4">
         <f t="shared" si="42"/>
-        <v>31761893.272774059</v>
+        <v>7627582.4694047505</v>
       </c>
       <c r="ER13" s="4">
         <f t="shared" si="42"/>
-        <v>34811035.026960373</v>
+        <v>8237789.066957131</v>
       </c>
       <c r="ES13" s="4">
         <f t="shared" si="42"/>
-        <v>38152894.38954857</v>
+        <v>8896812.1923137028</v>
       </c>
       <c r="ET13" s="4">
         <f t="shared" si="42"/>
-        <v>41815572.250945233</v>
+        <v>9608557.1676987987</v>
       </c>
       <c r="EU13" s="4">
         <f t="shared" si="42"/>
-        <v>45829867.187035978</v>
+        <v>10377241.741114704</v>
       </c>
       <c r="EV13" s="4">
         <f t="shared" si="42"/>
-        <v>50229534.436991438</v>
+        <v>11207421.080403881</v>
       </c>
       <c r="EW13" s="4">
         <f t="shared" si="42"/>
-        <v>55051569.742942624</v>
+        <v>12104014.766836192</v>
       </c>
       <c r="EX13" s="4">
         <f t="shared" si="42"/>
-        <v>60336520.438265122</v>
+        <v>13072335.948183089</v>
       </c>
       <c r="EY13" s="4">
         <f t="shared" si="42"/>
-        <v>66128826.400338583</v>
+        <v>14118122.824037738</v>
       </c>
       <c r="EZ13" s="4">
         <f t="shared" si="42"/>
-        <v>72477193.734771088</v>
+        <v>15247572.649960758</v>
       </c>
       <c r="FA13" s="4">
         <f t="shared" si="42"/>
-        <v>79435004.333309114</v>
+        <v>16467378.46195762</v>
       </c>
       <c r="FB13" s="4">
         <f t="shared" si="42"/>
-        <v>87060764.749306798</v>
+        <v>17784768.738914233</v>
       </c>
       <c r="FC13" s="4">
         <f t="shared" si="42"/>
-        <v>95418598.165240258</v>
+        <v>19207550.238027371</v>
       </c>
       <c r="FD13" s="4">
         <f t="shared" si="42"/>
-        <v>104578783.58910333</v>
+        <v>20744154.257069562</v>
       </c>
       <c r="FE13" s="4">
         <f t="shared" si="42"/>
-        <v>114618346.81365725</v>
+        <v>22403686.597635128</v>
       </c>
       <c r="FF13" s="4">
         <f t="shared" si="42"/>
-        <v>125621708.10776836</v>
+        <v>24195981.525445938</v>
       </c>
       <c r="FG13" s="4">
         <f t="shared" si="42"/>
-        <v>137681392.08611414</v>
+        <v>26131660.047481615</v>
       </c>
       <c r="FH13" s="4">
         <f t="shared" si="42"/>
-        <v>150898805.72638109</v>
+        <v>28222192.851280145</v>
       </c>
     </row>
     <row r="14" spans="1:164" x14ac:dyDescent="0.25">
@@ -3134,7 +3274,7 @@
       </c>
       <c r="AI14" s="10">
         <f>AI13/AI12-1</f>
-        <v>-9.777700336777051E-3</v>
+        <v>-0.67351205495937361</v>
       </c>
       <c r="AJ14" s="4"/>
       <c r="AK14" s="4"/>
@@ -3514,7 +3654,7 @@
         <v>-1.4132352941176469</v>
       </c>
       <c r="AC19" s="7">
-        <f t="shared" si="43"/>
+        <f>AC13/AB13-1</f>
         <v>-8.270462633451956</v>
       </c>
       <c r="AD19" s="7">

</xml_diff>